<commit_message>
updated added to addProviderCodeInformation
</commit_message>
<xml_diff>
--- a/InsuranceNow_v1.0/testData/providerData.xlsx
+++ b/InsuranceNow_v1.0/testData/providerData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srajendran\git\seleniumJavaRepo\InsuranceNow_v1.0\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8405DF2D-7BEF-4C77-954F-2AD3A6035CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DED198D-D1D7-4888-98DD-B7CACCB099C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{838B1716-2769-449B-83C2-A98D2BE273E4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>First Name</t>
   </si>
@@ -60,64 +60,28 @@
     <t>password</t>
   </si>
   <si>
-    <t>ADJ I</t>
-  </si>
-  <si>
-    <t>Kristal Fisher</t>
-  </si>
-  <si>
-    <t>Hillary Rape</t>
-  </si>
-  <si>
     <t>November@2024!</t>
   </si>
   <si>
-    <t>Helen</t>
-  </si>
-  <si>
-    <t>Kebede</t>
-  </si>
-  <si>
-    <t>689 262 7223</t>
-  </si>
-  <si>
-    <t>W854695</t>
-  </si>
-  <si>
-    <t>hkebede@ottersolv.com</t>
-  </si>
-  <si>
-    <t>Lesly Dorcely</t>
-  </si>
-  <si>
-    <t>Delonica</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>689 262 7228</t>
-  </si>
-  <si>
-    <t>G183277</t>
-  </si>
-  <si>
-    <t>djames@ottersolv.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ashley </t>
-  </si>
-  <si>
-    <t>Hillman</t>
-  </si>
-  <si>
-    <t>689 262 7229</t>
-  </si>
-  <si>
-    <t>W905068</t>
-  </si>
-  <si>
-    <t>ahillman@ottersolv.com</t>
+    <t>Jennifer</t>
+  </si>
+  <si>
+    <t>Freise</t>
+  </si>
+  <si>
+    <t>901-237-5634</t>
+  </si>
+  <si>
+    <t>W114228</t>
+  </si>
+  <si>
+    <t>Jennifer.Freise@sedgwick.com</t>
+  </si>
+  <si>
+    <t>Don Freihoefer</t>
+  </si>
+  <si>
+    <t>ADJ II</t>
   </si>
 </sst>
 </file>
@@ -202,15 +166,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -526,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4C1CEF3-1EB1-498B-ABFA-BD26A2AA477F}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,100 +546,38 @@
         <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="G2" s="4">
+        <v>45900</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="I2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="J2" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="G2" s="4">
-        <v>46660</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{046DC254-C4A1-4DB9-BFFE-71428513D6B5}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{052282E5-FE54-41CE-8D6D-C8255855C6BC}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{6B076531-60C3-4EDD-A642-A7D711B3480E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>